<commit_message>
expected num jobs created
</commit_message>
<xml_diff>
--- a/List_of_cites/Canada.xlsx
+++ b/List_of_cites/Canada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aujla\Downloads\Job_Search_Automation\List_of_cites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80BABEAF-F33F-4D4A-B22A-4C8AD7C31F51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D59BBA5-F847-4D1C-8A5E-D1A02B00F519}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5A94EBC4-9AD4-4FF1-B374-D76BBAE56C4E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="113">
   <si>
     <t>Toronto</t>
   </si>
@@ -737,7 +737,7 @@
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,6 +813,9 @@
       <c r="A7" t="s">
         <v>110</v>
       </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="2"/>

</xml_diff>

<commit_message>
expected vs actual jobs completed
</commit_message>
<xml_diff>
--- a/List_of_cites/Canada.xlsx
+++ b/List_of_cites/Canada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aujla\Downloads\Job_Search_Automation\List_of_cites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D59BBA5-F847-4D1C-8A5E-D1A02B00F519}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE7A92E-89B4-45B0-AA7C-2320A1A55678}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5A94EBC4-9AD4-4FF1-B374-D76BBAE56C4E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="112">
   <si>
     <t>Toronto</t>
   </si>
@@ -344,27 +344,9 @@
     <t>Innisfil</t>
   </si>
   <si>
-    <t>St. Catharines–Niagara Falls</t>
-  </si>
-  <si>
-    <t>Chicoutimi–Jonquière</t>
-  </si>
-  <si>
-    <t>Welland–Pelham</t>
-  </si>
-  <si>
-    <t>Alberta/Saskatchewan</t>
-  </si>
-  <si>
     <t>Cape Breton–Sydney</t>
   </si>
   <si>
-    <t>Keswick–Elmhurst Beach</t>
-  </si>
-  <si>
-    <t>Quispamsis–Rothesay</t>
-  </si>
-  <si>
     <t>Ottawa</t>
   </si>
   <si>
@@ -372,6 +354,21 @@
   </si>
   <si>
     <t>State</t>
+  </si>
+  <si>
+    <t>St. Catharines</t>
+  </si>
+  <si>
+    <t>Jonquière</t>
+  </si>
+  <si>
+    <t>Welland</t>
+  </si>
+  <si>
+    <t>Rothesay</t>
+  </si>
+  <si>
+    <t>Elmhurst Beach</t>
   </si>
 </sst>
 </file>
@@ -736,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9873BFED-42A1-4667-9538-6FC9019CF6E6}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,10 +745,10 @@
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -811,7 +808,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -931,7 +928,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
@@ -1063,7 +1060,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
@@ -1305,7 +1302,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B52" t="s">
         <v>1</v>
@@ -1671,7 +1668,7 @@
         <v>89</v>
       </c>
       <c r="B85" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -1712,7 +1709,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B89" t="s">
         <v>17</v>
@@ -1778,7 +1775,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B95" t="s">
         <v>1</v>
@@ -1822,7 +1819,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B99" t="s">
         <v>34</v>

</xml_diff>